<commit_message>
Still not done with achievements
</commit_message>
<xml_diff>
--- a/Planning/Achievements.xlsx
+++ b/Planning/Achievements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Simonsen\Documents\GitHub\Pingu\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielSimonsen\source\repos\Pingu\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42B906D-CEEA-4D49-9D15-29A3705CB963}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E8BE42-E0F7-4E4F-A18A-5C9C094451AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -716,19 +716,72 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -775,11 +828,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1078,8 +1143,8 @@
   <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,8 +1901,8 @@
       </c>
     </row>
     <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="15"/>
-      <c r="B96" s="11" t="s">
+      <c r="A96" s="14"/>
+      <c r="B96" s="10" t="s">
         <v>64</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -1845,10 +1910,10 @@
       </c>
     </row>
     <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+      <c r="A97" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="17" t="s">
         <v>158</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -1856,20 +1921,20 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="16"/>
-      <c r="B98" s="2" t="s">
+      <c r="A98" s="18"/>
+      <c r="B98" s="19" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="16"/>
-      <c r="B99" s="2" t="s">
+      <c r="A99" s="18"/>
+      <c r="B99" s="19" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="16"/>
-      <c r="B100" s="2" t="s">
+      <c r="A100" s="18"/>
+      <c r="B100" s="19" t="s">
         <v>160</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -1877,8 +1942,8 @@
       </c>
     </row>
     <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="16"/>
-      <c r="B101" s="2" t="s">
+      <c r="A101" s="18"/>
+      <c r="B101" s="19" t="s">
         <v>161</v>
       </c>
       <c r="E101" s="1" t="s">
@@ -1886,8 +1951,8 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="16"/>
-      <c r="B102" s="2" t="s">
+      <c r="A102" s="18"/>
+      <c r="B102" s="19" t="s">
         <v>61</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -1895,8 +1960,8 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="16"/>
-      <c r="B103" s="2" t="s">
+      <c r="A103" s="18"/>
+      <c r="B103" s="19" t="s">
         <v>168</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -1904,15 +1969,17 @@
       </c>
     </row>
     <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B104" s="2" t="s">
+      <c r="A104" s="18"/>
+      <c r="B104" s="19" t="s">
         <v>169</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B105" s="2" t="s">
+    <row r="105" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="20"/>
+      <c r="B105" s="21" t="s">
         <v>165</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -1925,7 +1992,7 @@
     <mergeCell ref="A85:A88"/>
     <mergeCell ref="A89:A96"/>
     <mergeCell ref="A3:A51"/>
-    <mergeCell ref="A97:A103"/>
+    <mergeCell ref="A97:A105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Achievements gets added to db
</commit_message>
<xml_diff>
--- a/Planning/Achievements.xlsx
+++ b/Planning/Achievements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielSimonsen\source\repos\Pingu\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Simonsen\Documents\GitHub\Pingu\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E8BE42-E0F7-4E4F-A18A-5C9C094451AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C422DE6B-3D35-460D-B34E-6659E7F727E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -831,20 +831,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1143,8 +1143,8 @@
   <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,7 +1913,7 @@
       <c r="A97" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="19" t="s">
         <v>158</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -1921,20 +1921,20 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="18"/>
-      <c r="B98" s="19" t="s">
+      <c r="A98" s="17"/>
+      <c r="B98" s="20" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="18"/>
-      <c r="B99" s="19" t="s">
+      <c r="A99" s="17"/>
+      <c r="B99" s="20" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19" t="s">
+      <c r="A100" s="17"/>
+      <c r="B100" s="20" t="s">
         <v>160</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -1942,8 +1942,8 @@
       </c>
     </row>
     <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="18"/>
-      <c r="B101" s="19" t="s">
+      <c r="A101" s="17"/>
+      <c r="B101" s="20" t="s">
         <v>161</v>
       </c>
       <c r="E101" s="1" t="s">
@@ -1951,8 +1951,8 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="18"/>
-      <c r="B102" s="19" t="s">
+      <c r="A102" s="17"/>
+      <c r="B102" s="20" t="s">
         <v>61</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -1960,8 +1960,8 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="18"/>
-      <c r="B103" s="19" t="s">
+      <c r="A103" s="17"/>
+      <c r="B103" s="20" t="s">
         <v>168</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -1969,8 +1969,8 @@
       </c>
     </row>
     <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="18"/>
-      <c r="B104" s="19" t="s">
+      <c r="A104" s="17"/>
+      <c r="B104" s="20" t="s">
         <v>169</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -1978,7 +1978,7 @@
       </c>
     </row>
     <row r="105" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="20"/>
+      <c r="A105" s="18"/>
       <c r="B105" s="21" t="s">
         <v>165</v>
       </c>

</xml_diff>